<commit_message>
[Not working] Changed tables
</commit_message>
<xml_diff>
--- a/data/tables/paradigms_nouns.xlsx
+++ b/data/tables/paradigms_nouns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgcha\Desktop\Python\Códigos\tsakonian_dictionary_app\data\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8432AE84-432C-4611-9C69-5FF51CA9C51D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C29D22B-0860-4F4E-A958-EFD488B4774D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1026,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>